<commit_message>
changes template file load-faults module and fix bugs tildes to download file
</commit_message>
<xml_diff>
--- a/src/assets/documents/Template-BasePymes-FallasRR.xlsx
+++ b/src/assets/documents/Template-BasePymes-FallasRR.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EUDY\Desktop\Plantillas - Fallas RR\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FE37B693-C003-4538-915B-3CA4F6A4F423}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4335" yWindow="2610" windowWidth="16770" windowHeight="8265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="MATRIZ" sheetId="1" r:id="rId1"/>
@@ -52,13 +46,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;$&quot;\ * #,##0_-;\-&quot;$&quot;\ * #,##0_-;_-&quot;$&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;$&quot;\ * #,##0.00_-;\-&quot;$&quot;\ * #,##0.00_-;_-&quot;$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,14 +80,6 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -109,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -156,24 +142,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -187,16 +164,12 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="% 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Millares 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Moneda [0] 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Moneda 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="% 2" xfId="4"/>
+    <cellStyle name="Millares 2" xfId="1"/>
+    <cellStyle name="Moneda [0] 2" xfId="3"/>
+    <cellStyle name="Moneda 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -204,9 +177,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -255,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -288,26 +258,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -340,23 +293,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,10 +468,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -566,22 +504,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="6"/>
-      <c r="E2" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -605,22 +539,18 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -648,20 +578,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -689,10 +617,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>